<commit_message>
ispravil kalibrovku s perenosom rascheta korrekcii nizkoj temperatury v kalibrovochnyj xls fajl;
</commit_message>
<xml_diff>
--- a/calibration_calculator.xlsx
+++ b/calibration_calculator.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t>№</t>
   </si>
@@ -41,6 +41,9 @@
   <si>
     <t>50⁰C</t>
   </si>
+  <si>
+    <t>rectal</t>
+  </si>
 </sst>
 </file>
 
@@ -49,7 +52,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,6 +60,20 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE181E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF4000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -79,10 +96,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -377,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X47"/>
+  <dimension ref="A1:X48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1299,6 +1318,35 @@
         <v>0.05</v>
       </c>
     </row>
+    <row r="18" spans="1:24">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3">
+        <v>-4.54</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="D18" s="4">
+        <v>5.12</v>
+      </c>
+      <c r="E18" s="4">
+        <v>9.75</v>
+      </c>
+      <c r="F18" s="4">
+        <v>10.06</v>
+      </c>
+      <c r="G18">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="H18">
+        <v>30</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
     <row r="19" spans="1:24">
       <c r="A19" s="1">
         <f>B19-$B$1</f>
@@ -1391,7 +1439,7 @@
     </row>
     <row r="20" spans="1:24">
       <c r="A20" s="1">
-        <f t="shared" ref="A20:A32" si="2">B20-$B$1</f>
+        <f t="shared" ref="A20:A33" si="2">B20-$B$1</f>
         <v>0.15000000000000036</v>
       </c>
       <c r="B20" s="1">
@@ -1431,11 +1479,11 @@
         <v>49.989999999999995</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" ref="K20:K32" si="4">A20/15</f>
+        <f t="shared" ref="K20:K33" si="4">A20/15</f>
         <v>1.0000000000000024E-2</v>
       </c>
       <c r="N20" s="1">
-        <f t="shared" ref="N20:N32" si="5">O20-$B$1</f>
+        <f t="shared" ref="N20:N31" si="5">O20-$B$1</f>
         <v>9.9999999999999645E-2</v>
       </c>
       <c r="O20" s="1">
@@ -1475,7 +1523,7 @@
         <v>50</v>
       </c>
       <c r="X20" s="2">
-        <f t="shared" ref="X20:X32" si="7">N20/15</f>
+        <f t="shared" ref="X20:X31" si="7">N20/15</f>
         <v>6.6666666666666428E-3</v>
       </c>
     </row>
@@ -2303,7 +2351,7 @@
         <v>0.11000000000000032</v>
       </c>
       <c r="B32" s="1">
-        <f t="shared" ref="B32:J32" si="26">B17-$K17</f>
+        <f t="shared" ref="B32:J33" si="26">B17-$K17</f>
         <v>-4.8899999999999997</v>
       </c>
       <c r="C32" s="1">
@@ -2344,9 +2392,55 @@
       </c>
       <c r="X32" s="2"/>
     </row>
-    <row r="34" spans="2:19">
+    <row r="33" spans="1:19">
+      <c r="A33" s="1">
+        <f t="shared" si="2"/>
+        <v>0.41000000000000014</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="26"/>
+        <v>-4.59</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" si="26"/>
+        <v>0.18</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="26"/>
+        <v>5.07</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="26"/>
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="26"/>
+        <v>10.01</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="26"/>
+        <v>19.96</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="26"/>
+        <v>29.95</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" si="26"/>
+        <v>-0.05</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" si="26"/>
+        <v>-0.05</v>
+      </c>
+      <c r="K33" s="2">
+        <f t="shared" si="4"/>
+        <v>2.7333333333333341E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
       <c r="B34" s="1">
-        <f t="shared" ref="B34:E34" si="27">B19-(10-B19)*$K19</f>
+        <f t="shared" ref="B34:F35" si="27">B19-(10-B19)*$K19</f>
         <v>-4.9982933333333337</v>
       </c>
       <c r="C34" s="1">
@@ -2362,11 +2456,11 @@
         <v>9.7372266666666647</v>
       </c>
       <c r="F34" s="1">
-        <f>F19-(10-F19)*$K19</f>
+        <f t="shared" si="27"/>
         <v>10.040426666666665</v>
       </c>
       <c r="O34" s="1">
-        <f t="shared" ref="O34:R34" si="28">O19-(10-O19)*$X19</f>
+        <f t="shared" ref="O34:S35" si="28">O19-(10-O19)*$X19</f>
         <v>-4.9997600000000002</v>
       </c>
       <c r="P34" s="1">
@@ -2382,450 +2476,472 @@
         <v>9.6887600000000003</v>
       </c>
       <c r="S34" s="1">
-        <f>S19-(10-S19)*$X19</f>
+        <f t="shared" si="28"/>
         <v>9.98996</v>
       </c>
     </row>
-    <row r="35" spans="2:19">
+    <row r="35" spans="1:19">
       <c r="B35" s="1">
-        <f t="shared" ref="B35:F35" si="29">B20-(10-B20)*$K20</f>
+        <f t="shared" si="27"/>
         <v>-4.9984999999999999</v>
       </c>
       <c r="C35" s="1">
+        <f t="shared" si="27"/>
+        <v>9.9999999999976497E-4</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="27"/>
+        <v>5.0106000000000002</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="27"/>
+        <v>9.7272999999999996</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="27"/>
+        <v>10.030299999999999</v>
+      </c>
+      <c r="O35" s="1">
+        <f t="shared" si="28"/>
+        <v>-4.9993333333333334</v>
+      </c>
+      <c r="P35" s="1">
+        <f t="shared" si="28"/>
+        <v>-6.2666666666664345E-3</v>
+      </c>
+      <c r="Q35" s="1">
+        <f t="shared" si="28"/>
+        <v>4.9867999999999997</v>
+      </c>
+      <c r="R35" s="1">
+        <f t="shared" si="28"/>
+        <v>9.6979999999999986</v>
+      </c>
+      <c r="S35" s="1">
+        <f t="shared" si="28"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
+      <c r="B37" s="1">
+        <f t="shared" ref="B37:F39" si="29">B22-(10-B22)*$K22</f>
+        <v>-4.9984999999999999</v>
+      </c>
+      <c r="C37" s="1">
         <f t="shared" si="29"/>
         <v>9.9999999999976497E-4</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D37" s="1">
         <f t="shared" si="29"/>
+        <v>5.0207000000000006</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="29"/>
+        <v>9.7374000000000009</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="29"/>
+        <v>10.040400000000002</v>
+      </c>
+      <c r="O37" s="1">
+        <f t="shared" ref="O37:S39" si="30">O22-(10-O22)*$X22</f>
+        <v>-4.9990399999999999</v>
+      </c>
+      <c r="P37" s="1">
+        <f t="shared" si="30"/>
+        <v>6.3999999999991841E-4</v>
+      </c>
+      <c r="Q37" s="1">
+        <f t="shared" si="30"/>
+        <v>5.0003200000000003</v>
+      </c>
+      <c r="R37" s="1">
+        <f t="shared" si="30"/>
+        <v>9.7076799999999999</v>
+      </c>
+      <c r="S37" s="1">
+        <f t="shared" si="30"/>
+        <v>10.020159999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
+      <c r="B38" s="1">
+        <f t="shared" si="29"/>
+        <v>-4.9998933333333335</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" si="29"/>
+        <v>-2.6666666666666693E-2</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="29"/>
+        <v>4.966613333333334</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="29"/>
+        <v>9.6791466666666661</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="29"/>
+        <v>9.979946666666665</v>
+      </c>
+      <c r="O38" s="1">
+        <f t="shared" si="30"/>
+        <v>-4.9995733333333332</v>
+      </c>
+      <c r="P38" s="1">
+        <f t="shared" si="30"/>
+        <v>-1.3120000000000048E-2</v>
+      </c>
+      <c r="Q38" s="1">
+        <f t="shared" si="30"/>
+        <v>4.9833866666666662</v>
+      </c>
+      <c r="R38" s="1">
+        <f t="shared" si="30"/>
+        <v>9.688346666666666</v>
+      </c>
+      <c r="S38" s="1">
+        <f t="shared" si="30"/>
+        <v>9.9899466666666665</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="B39" s="1">
+        <f t="shared" si="29"/>
+        <v>-4.9982933333333337</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="29"/>
+        <v>-5.6000000000000633E-3</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="29"/>
+        <v>5.0174133333333337</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="29"/>
+        <v>9.7271200000000011</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="29"/>
+        <v>10.030320000000001</v>
+      </c>
+      <c r="O39" s="1">
+        <f t="shared" si="30"/>
+        <v>-4.9990399999999999</v>
+      </c>
+      <c r="P39" s="1">
+        <f t="shared" si="30"/>
+        <v>6.4000000000052903E-4</v>
+      </c>
+      <c r="Q39" s="1">
+        <f t="shared" si="30"/>
+        <v>5.0003200000000003</v>
+      </c>
+      <c r="R39" s="1">
+        <f t="shared" si="30"/>
+        <v>9.7076799999999999</v>
+      </c>
+      <c r="S39" s="1">
+        <f t="shared" si="30"/>
+        <v>10.01008</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
+      <c r="B41" s="1">
+        <f t="shared" ref="B41:F48" si="31">B26-(10-B26)*$K26</f>
+        <v>-4.9990399999999999</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="31"/>
+        <v>-1.9519999999999482E-2</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="31"/>
+        <v>5.0003200000000003</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="31"/>
+        <v>9.7076799999999999</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="31"/>
+        <v>10</v>
+      </c>
+      <c r="O41" s="1">
+        <f t="shared" ref="O41:S46" si="32">O26-(10-O26)*$X26</f>
+        <v>-4.9984999999999999</v>
+      </c>
+      <c r="P41" s="1">
+        <f t="shared" si="32"/>
+        <v>1.0000000000003617E-3</v>
+      </c>
+      <c r="Q41" s="1">
+        <f t="shared" si="32"/>
         <v>5.0106000000000002</v>
       </c>
-      <c r="E35" s="1">
-        <f t="shared" si="29"/>
+      <c r="R41" s="1">
+        <f t="shared" si="32"/>
         <v>9.7272999999999996</v>
       </c>
-      <c r="F35" s="1">
-        <f t="shared" si="29"/>
-        <v>10.030299999999999</v>
-      </c>
-      <c r="O35" s="1">
-        <f t="shared" ref="O35:S35" si="30">O20-(10-O20)*$X20</f>
+      <c r="S41" s="1">
+        <f t="shared" si="32"/>
+        <v>10.020199999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
+      <c r="B42" s="1">
+        <f t="shared" si="31"/>
+        <v>-4.9991933333333334</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="31"/>
+        <v>-2.820000000000239E-3</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="31"/>
+        <v>5.0137</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="31"/>
+        <v>9.7179466666666681</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="31"/>
+        <v>10.020146666666665</v>
+      </c>
+      <c r="O42" s="1">
+        <f t="shared" si="32"/>
+        <v>-4.99946</v>
+      </c>
+      <c r="P42" s="1">
+        <f t="shared" si="32"/>
+        <v>3.5999999999950655E-4</v>
+      </c>
+      <c r="Q42" s="1">
+        <f t="shared" si="32"/>
+        <v>5.0001800000000003</v>
+      </c>
+      <c r="R42" s="1">
+        <f t="shared" si="32"/>
+        <v>9.6981999999999999</v>
+      </c>
+      <c r="S42" s="1">
+        <f t="shared" si="32"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
+      <c r="B43" s="1">
+        <f t="shared" si="31"/>
+        <v>-4.99946</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="31"/>
+        <v>-1.9759999999999903E-2</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="31"/>
+        <v>4.9901199999999992</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="31"/>
+        <v>9.6982000000000017</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="31"/>
+        <v>10</v>
+      </c>
+      <c r="O43" s="1">
+        <f t="shared" si="32"/>
+        <v>-4.9998933333333335</v>
+      </c>
+      <c r="P43" s="1">
+        <f t="shared" si="32"/>
+        <v>-1.6640000000000016E-2</v>
+      </c>
+      <c r="Q43" s="1">
+        <f t="shared" si="32"/>
+        <v>4.9766399999999997</v>
+      </c>
+      <c r="R43" s="1">
+        <f t="shared" si="32"/>
+        <v>9.6691199999999995</v>
+      </c>
+      <c r="S43" s="1">
+        <f t="shared" si="32"/>
+        <v>9.9699199999999983</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="B44" s="1">
+        <f t="shared" si="31"/>
+        <v>-4.9991933333333334</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="31"/>
+        <v>-2.8199999999996145E-3</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="31"/>
+        <v>5.0036266666666673</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="31"/>
+        <v>9.7078733333333318</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="31"/>
+        <v>10.010073333333333</v>
+      </c>
+      <c r="O44" s="1">
+        <f t="shared" si="32"/>
+        <v>-4.999673333333333</v>
+      </c>
+      <c r="P44" s="1">
+        <f t="shared" si="32"/>
+        <v>-6.4800000000001801E-3</v>
+      </c>
+      <c r="Q44" s="1">
+        <f t="shared" si="32"/>
+        <v>4.9967599999999992</v>
+      </c>
+      <c r="R44" s="1">
+        <f t="shared" si="32"/>
+        <v>9.6885533333333331</v>
+      </c>
+      <c r="S44" s="1">
+        <f t="shared" si="32"/>
+        <v>9.9899533333333341</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
+      <c r="B45" s="1">
+        <f t="shared" si="31"/>
+        <v>-4.99946</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" si="31"/>
+        <v>-9.6999999999999101E-3</v>
+      </c>
+      <c r="D45" s="1">
+        <f t="shared" si="31"/>
+        <v>5.0102400000000005</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="31"/>
+        <v>9.708260000000001</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="31"/>
+        <v>10.010059999999999</v>
+      </c>
+      <c r="O45" s="1">
+        <f t="shared" si="32"/>
+        <v>-4.999673333333333</v>
+      </c>
+      <c r="P45" s="1">
+        <f t="shared" si="32"/>
+        <v>-6.4799999999996111E-3</v>
+      </c>
+      <c r="Q45" s="1">
+        <f t="shared" si="32"/>
+        <v>4.9967600000000001</v>
+      </c>
+      <c r="R45" s="1">
+        <f t="shared" si="32"/>
+        <v>9.6986000000000008</v>
+      </c>
+      <c r="S45" s="1">
+        <f t="shared" si="32"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
+      <c r="B46" s="1">
+        <f t="shared" si="31"/>
+        <v>-4.9995733333333332</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" si="31"/>
+        <v>-1.3120000000000062E-2</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" si="31"/>
+        <v>4.9934399999999997</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="31"/>
+        <v>9.6983999999999995</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="31"/>
+        <v>10</v>
+      </c>
+      <c r="O46" s="1">
+        <f t="shared" si="32"/>
         <v>-4.9993333333333334</v>
       </c>
-      <c r="P35" s="1">
-        <f t="shared" si="30"/>
+      <c r="P46" s="1">
+        <f t="shared" si="32"/>
         <v>-6.2666666666664345E-3</v>
       </c>
-      <c r="Q35" s="1">
-        <f t="shared" si="30"/>
-        <v>4.9867999999999997</v>
-      </c>
-      <c r="R35" s="1">
-        <f t="shared" si="30"/>
+      <c r="Q46" s="1">
+        <f t="shared" si="32"/>
+        <v>5.0069333333333335</v>
+      </c>
+      <c r="R46" s="1">
+        <f t="shared" si="32"/>
         <v>9.6979999999999986</v>
       </c>
-      <c r="S35" s="1">
-        <f t="shared" si="30"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="2:19">
-      <c r="B37" s="1">
-        <f t="shared" ref="B37:F37" si="31">B22-(10-B22)*$K22</f>
-        <v>-4.9984999999999999</v>
-      </c>
-      <c r="C37" s="1">
-        <f t="shared" si="31"/>
-        <v>9.9999999999976497E-4</v>
-      </c>
-      <c r="D37" s="1">
-        <f t="shared" si="31"/>
-        <v>5.0207000000000006</v>
-      </c>
-      <c r="E37" s="1">
-        <f t="shared" si="31"/>
-        <v>9.7374000000000009</v>
-      </c>
-      <c r="F37" s="1">
-        <f t="shared" si="31"/>
-        <v>10.040400000000002</v>
-      </c>
-      <c r="O37" s="1">
-        <f t="shared" ref="O37:S37" si="32">O22-(10-O22)*$X22</f>
-        <v>-4.9990399999999999</v>
-      </c>
-      <c r="P37" s="1">
+      <c r="S46" s="1">
         <f t="shared" si="32"/>
-        <v>6.3999999999991841E-4</v>
-      </c>
-      <c r="Q37" s="1">
-        <f t="shared" si="32"/>
-        <v>5.0003200000000003</v>
-      </c>
-      <c r="R37" s="1">
-        <f t="shared" si="32"/>
-        <v>9.7076799999999999</v>
-      </c>
-      <c r="S37" s="1">
-        <f t="shared" si="32"/>
-        <v>10.020159999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="2:19">
-      <c r="B38" s="1">
-        <f t="shared" ref="B38:F38" si="33">B23-(10-B23)*$K23</f>
-        <v>-4.9998933333333335</v>
-      </c>
-      <c r="C38" s="1">
-        <f t="shared" si="33"/>
-        <v>-2.6666666666666693E-2</v>
-      </c>
-      <c r="D38" s="1">
-        <f t="shared" si="33"/>
-        <v>4.966613333333334</v>
-      </c>
-      <c r="E38" s="1">
-        <f t="shared" si="33"/>
-        <v>9.6791466666666661</v>
-      </c>
-      <c r="F38" s="1">
-        <f t="shared" si="33"/>
-        <v>9.979946666666665</v>
-      </c>
-      <c r="O38" s="1">
-        <f t="shared" ref="O38:S38" si="34">O23-(10-O23)*$X23</f>
-        <v>-4.9995733333333332</v>
-      </c>
-      <c r="P38" s="1">
-        <f t="shared" si="34"/>
-        <v>-1.3120000000000048E-2</v>
-      </c>
-      <c r="Q38" s="1">
-        <f t="shared" si="34"/>
-        <v>4.9833866666666662</v>
-      </c>
-      <c r="R38" s="1">
-        <f t="shared" si="34"/>
-        <v>9.688346666666666</v>
-      </c>
-      <c r="S38" s="1">
-        <f t="shared" si="34"/>
-        <v>9.9899466666666665</v>
-      </c>
-    </row>
-    <row r="39" spans="2:19">
-      <c r="B39" s="1">
-        <f t="shared" ref="B39:F39" si="35">B24-(10-B24)*$K24</f>
-        <v>-4.9982933333333337</v>
-      </c>
-      <c r="C39" s="1">
-        <f t="shared" si="35"/>
-        <v>-5.6000000000000633E-3</v>
-      </c>
-      <c r="D39" s="1">
-        <f t="shared" si="35"/>
-        <v>5.0174133333333337</v>
-      </c>
-      <c r="E39" s="1">
-        <f t="shared" si="35"/>
-        <v>9.7271200000000011</v>
-      </c>
-      <c r="F39" s="1">
-        <f t="shared" si="35"/>
-        <v>10.030320000000001</v>
-      </c>
-      <c r="O39" s="1">
-        <f t="shared" ref="O39:S39" si="36">O24-(10-O24)*$X24</f>
-        <v>-4.9990399999999999</v>
-      </c>
-      <c r="P39" s="1">
-        <f t="shared" si="36"/>
-        <v>6.4000000000052903E-4</v>
-      </c>
-      <c r="Q39" s="1">
-        <f t="shared" si="36"/>
-        <v>5.0003200000000003</v>
-      </c>
-      <c r="R39" s="1">
-        <f t="shared" si="36"/>
-        <v>9.7076799999999999</v>
-      </c>
-      <c r="S39" s="1">
-        <f t="shared" si="36"/>
-        <v>10.01008</v>
-      </c>
-    </row>
-    <row r="41" spans="2:19">
-      <c r="B41" s="1">
-        <f t="shared" ref="B41:F41" si="37">B26-(10-B26)*$K26</f>
-        <v>-4.9990399999999999</v>
-      </c>
-      <c r="C41" s="1">
-        <f t="shared" si="37"/>
-        <v>-1.9519999999999482E-2</v>
-      </c>
-      <c r="D41" s="1">
-        <f t="shared" si="37"/>
-        <v>5.0003200000000003</v>
-      </c>
-      <c r="E41" s="1">
-        <f t="shared" si="37"/>
-        <v>9.7076799999999999</v>
-      </c>
-      <c r="F41" s="1">
-        <f t="shared" si="37"/>
-        <v>10</v>
-      </c>
-      <c r="O41" s="1">
-        <f t="shared" ref="O41:S41" si="38">O26-(10-O26)*$X26</f>
-        <v>-4.9984999999999999</v>
-      </c>
-      <c r="P41" s="1">
-        <f t="shared" si="38"/>
-        <v>1.0000000000003617E-3</v>
-      </c>
-      <c r="Q41" s="1">
-        <f t="shared" si="38"/>
-        <v>5.0106000000000002</v>
-      </c>
-      <c r="R41" s="1">
-        <f t="shared" si="38"/>
-        <v>9.7272999999999996</v>
-      </c>
-      <c r="S41" s="1">
-        <f t="shared" si="38"/>
-        <v>10.020199999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="2:19">
-      <c r="B42" s="1">
-        <f t="shared" ref="B42:F42" si="39">B27-(10-B27)*$K27</f>
+        <v>10.010066666666667</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
+      <c r="B47" s="1">
+        <f t="shared" si="31"/>
         <v>-4.9991933333333334</v>
       </c>
-      <c r="C42" s="1">
-        <f t="shared" si="39"/>
-        <v>-2.820000000000239E-3</v>
-      </c>
-      <c r="D42" s="1">
-        <f t="shared" si="39"/>
-        <v>5.0137</v>
-      </c>
-      <c r="E42" s="1">
-        <f t="shared" si="39"/>
-        <v>9.7179466666666681</v>
-      </c>
-      <c r="F42" s="1">
-        <f t="shared" si="39"/>
-        <v>10.020146666666665</v>
-      </c>
-      <c r="O42" s="1">
-        <f t="shared" ref="O42:S42" si="40">O27-(10-O27)*$X27</f>
-        <v>-4.99946</v>
-      </c>
-      <c r="P42" s="1">
-        <f t="shared" si="40"/>
-        <v>3.5999999999950655E-4</v>
-      </c>
-      <c r="Q42" s="1">
-        <f t="shared" si="40"/>
-        <v>5.0001800000000003</v>
-      </c>
-      <c r="R42" s="1">
-        <f t="shared" si="40"/>
-        <v>9.6981999999999999</v>
-      </c>
-      <c r="S42" s="1">
-        <f t="shared" si="40"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="2:19">
-      <c r="B43" s="1">
-        <f t="shared" ref="B43:F43" si="41">B28-(10-B28)*$K28</f>
-        <v>-4.99946</v>
-      </c>
-      <c r="C43" s="1">
-        <f t="shared" si="41"/>
-        <v>-1.9759999999999903E-2</v>
-      </c>
-      <c r="D43" s="1">
-        <f t="shared" si="41"/>
-        <v>4.9901199999999992</v>
-      </c>
-      <c r="E43" s="1">
-        <f t="shared" si="41"/>
-        <v>9.6982000000000017</v>
-      </c>
-      <c r="F43" s="1">
-        <f t="shared" si="41"/>
-        <v>10</v>
-      </c>
-      <c r="O43" s="1">
-        <f t="shared" ref="O43:S43" si="42">O28-(10-O28)*$X28</f>
-        <v>-4.9998933333333335</v>
-      </c>
-      <c r="P43" s="1">
-        <f t="shared" si="42"/>
-        <v>-1.6640000000000016E-2</v>
-      </c>
-      <c r="Q43" s="1">
-        <f t="shared" si="42"/>
-        <v>4.9766399999999997</v>
-      </c>
-      <c r="R43" s="1">
-        <f t="shared" si="42"/>
-        <v>9.6691199999999995</v>
-      </c>
-      <c r="S43" s="1">
-        <f t="shared" si="42"/>
-        <v>9.9699199999999983</v>
-      </c>
-    </row>
-    <row r="44" spans="2:19">
-      <c r="B44" s="1">
-        <f t="shared" ref="B44:F44" si="43">B29-(10-B29)*$K29</f>
-        <v>-4.9991933333333334</v>
-      </c>
-      <c r="C44" s="1">
-        <f t="shared" si="43"/>
-        <v>-2.8199999999996145E-3</v>
-      </c>
-      <c r="D44" s="1">
-        <f t="shared" si="43"/>
-        <v>5.0036266666666673</v>
-      </c>
-      <c r="E44" s="1">
-        <f t="shared" si="43"/>
+      <c r="C47" s="1">
+        <f t="shared" si="31"/>
+        <v>-1.2893333333333548E-2</v>
+      </c>
+      <c r="D47" s="1">
+        <f t="shared" si="31"/>
+        <v>5.0036266666666664</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="31"/>
         <v>9.7078733333333318</v>
       </c>
-      <c r="F44" s="1">
-        <f t="shared" si="43"/>
+      <c r="F47" s="1">
+        <f t="shared" si="31"/>
         <v>10.010073333333333</v>
       </c>
-      <c r="O44" s="1">
-        <f t="shared" ref="O44:S44" si="44">O29-(10-O29)*$X29</f>
-        <v>-4.999673333333333</v>
-      </c>
-      <c r="P44" s="1">
-        <f t="shared" si="44"/>
-        <v>-6.4800000000001801E-3</v>
-      </c>
-      <c r="Q44" s="1">
-        <f t="shared" si="44"/>
-        <v>4.9967599999999992</v>
-      </c>
-      <c r="R44" s="1">
-        <f t="shared" si="44"/>
-        <v>9.6885533333333331</v>
-      </c>
-      <c r="S44" s="1">
-        <f t="shared" si="44"/>
-        <v>9.9899533333333341</v>
-      </c>
-    </row>
-    <row r="45" spans="2:19">
-      <c r="B45" s="1">
-        <f t="shared" ref="B45:F45" si="45">B30-(10-B30)*$K30</f>
-        <v>-4.99946</v>
-      </c>
-      <c r="C45" s="1">
-        <f t="shared" si="45"/>
-        <v>-9.6999999999999101E-3</v>
-      </c>
-      <c r="D45" s="1">
-        <f t="shared" si="45"/>
-        <v>5.0102400000000005</v>
-      </c>
-      <c r="E45" s="1">
-        <f t="shared" si="45"/>
-        <v>9.708260000000001</v>
-      </c>
-      <c r="F45" s="1">
-        <f t="shared" si="45"/>
-        <v>10.010059999999999</v>
-      </c>
-      <c r="O45" s="1">
-        <f t="shared" ref="O45:S45" si="46">O30-(10-O30)*$X30</f>
-        <v>-4.999673333333333</v>
-      </c>
-      <c r="P45" s="1">
-        <f t="shared" si="46"/>
-        <v>-6.4799999999996111E-3</v>
-      </c>
-      <c r="Q45" s="1">
-        <f t="shared" si="46"/>
-        <v>4.9967600000000001</v>
-      </c>
-      <c r="R45" s="1">
-        <f t="shared" si="46"/>
-        <v>9.6986000000000008</v>
-      </c>
-      <c r="S45" s="1">
-        <f t="shared" si="46"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="2:19">
-      <c r="B46" s="1">
-        <f t="shared" ref="B46:F46" si="47">B31-(10-B31)*$K31</f>
-        <v>-4.9995733333333332</v>
-      </c>
-      <c r="C46" s="1">
-        <f t="shared" si="47"/>
-        <v>-1.3120000000000062E-2</v>
-      </c>
-      <c r="D46" s="1">
-        <f t="shared" si="47"/>
-        <v>4.9934399999999997</v>
-      </c>
-      <c r="E46" s="1">
-        <f t="shared" si="47"/>
-        <v>9.6983999999999995</v>
-      </c>
-      <c r="F46" s="1">
-        <f t="shared" si="47"/>
-        <v>10</v>
-      </c>
-      <c r="O46" s="1">
-        <f t="shared" ref="O46:S46" si="48">O31-(10-O31)*$X31</f>
-        <v>-4.9993333333333334</v>
-      </c>
-      <c r="P46" s="1">
-        <f t="shared" si="48"/>
-        <v>-6.2666666666664345E-3</v>
-      </c>
-      <c r="Q46" s="1">
-        <f t="shared" si="48"/>
-        <v>5.0069333333333335</v>
-      </c>
-      <c r="R46" s="1">
-        <f t="shared" si="48"/>
-        <v>9.6979999999999986</v>
-      </c>
-      <c r="S46" s="1">
-        <f t="shared" si="48"/>
-        <v>10.010066666666667</v>
-      </c>
-    </row>
-    <row r="47" spans="2:19">
-      <c r="B47" s="1">
-        <f t="shared" ref="B47:F47" si="49">B32-(10-B32)*$K32</f>
-        <v>-4.9991933333333334</v>
-      </c>
-      <c r="C47" s="1">
-        <f t="shared" si="49"/>
-        <v>-1.2893333333333548E-2</v>
-      </c>
-      <c r="D47" s="1">
-        <f t="shared" si="49"/>
-        <v>5.0036266666666664</v>
-      </c>
-      <c r="E47" s="1">
-        <f t="shared" si="49"/>
-        <v>9.7078733333333318</v>
-      </c>
-      <c r="F47" s="1">
-        <f t="shared" si="49"/>
-        <v>10.010073333333333</v>
+    </row>
+    <row r="48" spans="1:19">
+      <c r="B48" s="1">
+        <f t="shared" si="31"/>
+        <v>-4.9887933333333336</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" si="31"/>
+        <v>-8.8413333333333455E-2</v>
+      </c>
+      <c r="D48" s="1">
+        <f t="shared" si="31"/>
+        <v>4.935246666666667</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="31"/>
+        <v>9.6917999999999989</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="31"/>
+        <v>10.010273333333332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working; production; real calibrated temperatures;
</commit_message>
<xml_diff>
--- a/calibration_calculator.xlsx
+++ b/calibration_calculator.xlsx
@@ -398,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1323,25 +1323,31 @@
         <v>8</v>
       </c>
       <c r="B18" s="3">
-        <v>-4.54</v>
+        <v>-4.57</v>
       </c>
       <c r="C18" s="3">
-        <v>0.23</v>
-      </c>
-      <c r="D18" s="4">
-        <v>5.12</v>
+        <v>0.26</v>
+      </c>
+      <c r="D18" s="3">
+        <v>5.13</v>
       </c>
       <c r="E18" s="4">
-        <v>9.75</v>
+        <v>9.77</v>
       </c>
       <c r="F18" s="4">
-        <v>10.06</v>
+        <v>10.07</v>
       </c>
       <c r="G18">
-        <v>20.010000000000002</v>
+        <v>20.02</v>
       </c>
       <c r="H18">
-        <v>30</v>
+        <v>29.99</v>
+      </c>
+      <c r="I18">
+        <v>39.97</v>
+      </c>
+      <c r="J18">
+        <v>50</v>
       </c>
       <c r="K18" s="1">
         <v>0</v>
@@ -2395,47 +2401,47 @@
     <row r="33" spans="1:19">
       <c r="A33" s="1">
         <f t="shared" si="2"/>
-        <v>0.45999999999999996</v>
+        <v>0.42999999999999972</v>
       </c>
       <c r="B33" s="1">
         <f t="shared" si="26"/>
-        <v>-4.54</v>
+        <v>-4.57</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" si="26"/>
-        <v>0.23</v>
+        <v>0.26</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="26"/>
-        <v>5.12</v>
+        <v>5.13</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" si="26"/>
-        <v>9.75</v>
+        <v>9.77</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" si="26"/>
-        <v>10.06</v>
+        <v>10.07</v>
       </c>
       <c r="G33" s="1">
         <f t="shared" si="26"/>
-        <v>20.010000000000002</v>
+        <v>20.02</v>
       </c>
       <c r="H33" s="1">
         <f t="shared" si="26"/>
-        <v>30</v>
+        <v>29.99</v>
       </c>
       <c r="I33" s="1">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>39.97</v>
       </c>
       <c r="J33" s="1">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K33" s="2">
         <f t="shared" si="4"/>
-        <v>3.0666666666666665E-2</v>
+        <v>2.8666666666666649E-2</v>
       </c>
     </row>
     <row r="34" spans="1:19">
@@ -2925,23 +2931,23 @@
     <row r="48" spans="1:19">
       <c r="B48" s="1">
         <f t="shared" si="31"/>
-        <v>-4.9858933333333333</v>
+        <v>-4.9876733333333334</v>
       </c>
       <c r="C48" s="1">
         <f t="shared" si="31"/>
-        <v>-6.9613333333333277E-2</v>
+        <v>-1.9213333333333138E-2</v>
       </c>
       <c r="D48" s="1">
         <f t="shared" si="31"/>
-        <v>4.9703466666666669</v>
+        <v>4.9903933333333335</v>
       </c>
       <c r="E48" s="1">
         <f t="shared" si="31"/>
-        <v>9.7423333333333328</v>
+        <v>9.7634066666666666</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" si="31"/>
-        <v>10.06184</v>
+        <v>10.072006666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>